<commit_message>
add script for get 10 words and learn everyday. marked first 10 words in xls.
</commit_message>
<xml_diff>
--- a/Longman_Communication_3000.xlsx
+++ b/Longman_Communication_3000.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3168" uniqueCount="3166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3178" uniqueCount="3176">
   <si>
     <t xml:space="preserve">a </t>
   </si>
@@ -9517,6 +9517,36 @@
   </si>
   <si>
     <t>zone</t>
+  </si>
+  <si>
+    <t>глубоко</t>
+  </si>
+  <si>
+    <t>страсть</t>
+  </si>
+  <si>
+    <t>комфорт</t>
+  </si>
+  <si>
+    <t>реклама</t>
+  </si>
+  <si>
+    <t>злой, испорченный</t>
+  </si>
+  <si>
+    <t>хранить, запоминать</t>
+  </si>
+  <si>
+    <t>обладать</t>
+  </si>
+  <si>
+    <t>поединок</t>
+  </si>
+  <si>
+    <t>личный</t>
+  </si>
+  <si>
+    <t>мертвый</t>
   </si>
 </sst>
 </file>
@@ -9567,7 +9597,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9583,9 +9613,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9623,7 +9653,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9695,7 +9725,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9845,17 +9875,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3168"/>
+  <dimension ref="A1:C3168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3168" sqref="B3168"/>
+    <sheetView tabSelected="1" topLeftCell="A704" workbookViewId="0">
+      <selection activeCell="C719" sqref="C719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -10242,7 +10273,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -10250,7 +10281,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -10258,7 +10289,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>51</v>
       </c>
@@ -10266,7 +10297,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>52</v>
       </c>
@@ -10274,7 +10305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>53</v>
       </c>
@@ -10282,7 +10313,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>54</v>
       </c>
@@ -10290,7 +10321,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>55</v>
       </c>
@@ -10298,7 +10329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>56</v>
       </c>
@@ -10306,7 +10337,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>57</v>
       </c>
@@ -10314,7 +10345,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>58</v>
       </c>
@@ -10322,15 +10353,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" s="1" t="s">
+        <v>3169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>60</v>
       </c>
@@ -10338,7 +10372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>61</v>
       </c>
@@ -10346,7 +10380,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>62</v>
       </c>
@@ -10354,7 +10388,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>63</v>
       </c>
@@ -10362,7 +10396,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>64</v>
       </c>
@@ -14082,7 +14116,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="529" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A529" s="2">
         <v>529</v>
       </c>
@@ -14090,7 +14124,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="530" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A530" s="2">
         <v>530</v>
       </c>
@@ -14098,7 +14132,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="531" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A531" s="2">
         <v>531</v>
       </c>
@@ -14106,7 +14140,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="532" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A532" s="2">
         <v>532</v>
       </c>
@@ -14114,7 +14148,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="533" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A533" s="2">
         <v>533</v>
       </c>
@@ -14122,7 +14156,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="534" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A534" s="2">
         <v>534</v>
       </c>
@@ -14130,7 +14164,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="535" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A535" s="2">
         <v>535</v>
       </c>
@@ -14138,7 +14172,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="536" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A536" s="2">
         <v>536</v>
       </c>
@@ -14146,7 +14180,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="537" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A537" s="2">
         <v>537</v>
       </c>
@@ -14154,7 +14188,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="538" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A538" s="2">
         <v>538</v>
       </c>
@@ -14162,7 +14196,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="539" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A539" s="2">
         <v>539</v>
       </c>
@@ -14170,7 +14204,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="540" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A540" s="2">
         <v>540</v>
       </c>
@@ -14178,15 +14212,18 @@
         <v>539</v>
       </c>
     </row>
-    <row r="541" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A541" s="2">
         <v>541</v>
       </c>
       <c r="B541" s="1" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="542" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C541" s="1" t="s">
+        <v>3168</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A542" s="2">
         <v>542</v>
       </c>
@@ -14194,7 +14231,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="543" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A543" s="2">
         <v>543</v>
       </c>
@@ -14202,7 +14239,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="544" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A544" s="2">
         <v>544</v>
       </c>
@@ -15490,7 +15527,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="705" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="705" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A705" s="2">
         <v>705</v>
       </c>
@@ -15498,7 +15535,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="706" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="706" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A706" s="2">
         <v>706</v>
       </c>
@@ -15506,7 +15543,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="707" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="707" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A707" s="2">
         <v>707</v>
       </c>
@@ -15514,7 +15551,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="708" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="708" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A708" s="2">
         <v>708</v>
       </c>
@@ -15522,7 +15559,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="709" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="709" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A709" s="2">
         <v>709</v>
       </c>
@@ -15530,7 +15567,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="710" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="710" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A710" s="2">
         <v>710</v>
       </c>
@@ -15538,7 +15575,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="711" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="711" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A711" s="2">
         <v>711</v>
       </c>
@@ -15546,7 +15583,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="712" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="712" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A712" s="2">
         <v>712</v>
       </c>
@@ -15554,7 +15591,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="713" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="713" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A713" s="2">
         <v>713</v>
       </c>
@@ -15562,7 +15599,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="714" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="714" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A714" s="2">
         <v>714</v>
       </c>
@@ -15570,7 +15607,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="715" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="715" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A715" s="2">
         <v>715</v>
       </c>
@@ -15578,7 +15615,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="716" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="716" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A716" s="2">
         <v>716</v>
       </c>
@@ -15586,7 +15623,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="717" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="717" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A717" s="2">
         <v>717</v>
       </c>
@@ -15594,7 +15631,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="718" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="718" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A718" s="2">
         <v>718</v>
       </c>
@@ -15602,15 +15639,18 @@
         <v>717</v>
       </c>
     </row>
-    <row r="719" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="719" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A719" s="2">
         <v>719</v>
       </c>
       <c r="B719" s="1" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="720" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C719" s="1" t="s">
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A720" s="2">
         <v>720</v>
       </c>
@@ -15618,7 +15658,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="721" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="721" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A721" s="2">
         <v>721</v>
       </c>
@@ -15626,7 +15666,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="722" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="722" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A722" s="2">
         <v>722</v>
       </c>
@@ -15634,7 +15674,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="723" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="723" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A723" s="2">
         <v>723</v>
       </c>
@@ -15642,7 +15682,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="724" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="724" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A724" s="2">
         <v>724</v>
       </c>
@@ -15650,7 +15690,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="725" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="725" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A725" s="2">
         <v>725</v>
       </c>
@@ -15658,7 +15698,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="726" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="726" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A726" s="2">
         <v>726</v>
       </c>
@@ -15666,7 +15706,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="727" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="727" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A727" s="2">
         <v>727</v>
       </c>
@@ -15674,7 +15714,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="728" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="728" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A728" s="2">
         <v>728</v>
       </c>
@@ -15682,7 +15722,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="729" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="729" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A729" s="2">
         <v>729</v>
       </c>
@@ -15690,7 +15730,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="730" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A730" s="2">
         <v>730</v>
       </c>
@@ -15698,7 +15738,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="731" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="731" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A731" s="2">
         <v>731</v>
       </c>
@@ -15706,7 +15746,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="732" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="732" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A732" s="2">
         <v>732</v>
       </c>
@@ -15714,7 +15754,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="733" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="733" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A733" s="2">
         <v>733</v>
       </c>
@@ -15722,7 +15762,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="734" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="734" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A734" s="2">
         <v>734</v>
       </c>
@@ -15730,15 +15770,18 @@
         <v>733</v>
       </c>
     </row>
-    <row r="735" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="735" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A735" s="2">
         <v>735</v>
       </c>
       <c r="B735" s="1" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="736" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C735" s="1" t="s">
+        <v>3166</v>
+      </c>
+    </row>
+    <row r="736" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A736" s="2">
         <v>736</v>
       </c>
@@ -23170,7 +23213,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="1665" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1665" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1665" s="2">
         <v>1665</v>
       </c>
@@ -23178,7 +23221,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="1666" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1666" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1666" s="2">
         <v>1666</v>
       </c>
@@ -23186,7 +23229,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="1667" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1667" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1667" s="2">
         <v>1667</v>
       </c>
@@ -23194,7 +23237,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="1668" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1668" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1668" s="2">
         <v>1668</v>
       </c>
@@ -23202,7 +23245,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="1669" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1669" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1669" s="2">
         <v>1669</v>
       </c>
@@ -23210,7 +23253,7 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="1670" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1670" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1670" s="2">
         <v>1670</v>
       </c>
@@ -23218,7 +23261,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="1671" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1671" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1671" s="2">
         <v>1671</v>
       </c>
@@ -23226,7 +23269,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="1672" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1672" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1672" s="2">
         <v>1672</v>
       </c>
@@ -23234,7 +23277,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="1673" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1673" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1673" s="2">
         <v>1673</v>
       </c>
@@ -23242,7 +23285,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="1674" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1674" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1674" s="2">
         <v>1674</v>
       </c>
@@ -23250,7 +23293,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="1675" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1675" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1675" s="2">
         <v>1675</v>
       </c>
@@ -23258,7 +23301,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="1676" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1676" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1676" s="2">
         <v>1676</v>
       </c>
@@ -23266,15 +23309,18 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="1677" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1677" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1677" s="2">
         <v>1677</v>
       </c>
       <c r="B1677" s="1" t="s">
         <v>1675</v>
       </c>
-    </row>
-    <row r="1678" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1677" s="1" t="s">
+        <v>3173</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1678" s="2">
         <v>1678</v>
       </c>
@@ -23282,7 +23328,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="1679" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1679" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1679" s="2">
         <v>1679</v>
       </c>
@@ -23290,7 +23336,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="1680" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1680" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1680" s="2">
         <v>1680</v>
       </c>
@@ -25602,7 +25648,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="1969" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1969" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1969" s="2">
         <v>1969</v>
       </c>
@@ -25610,7 +25656,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="1970" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1970" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1970" s="2">
         <v>1970</v>
       </c>
@@ -25618,7 +25664,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="1971" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1971" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1971" s="2">
         <v>1971</v>
       </c>
@@ -25626,7 +25672,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="1972" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1972" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1972" s="2">
         <v>1972</v>
       </c>
@@ -25634,7 +25680,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="1973" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1973" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1973" s="2">
         <v>1973</v>
       </c>
@@ -25642,7 +25688,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="1974" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1974" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1974" s="2">
         <v>1974</v>
       </c>
@@ -25650,7 +25696,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="1975" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1975" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1975" s="2">
         <v>1975</v>
       </c>
@@ -25658,7 +25704,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="1976" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1976" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1976" s="2">
         <v>1976</v>
       </c>
@@ -25666,15 +25712,18 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="1977" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1977" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1977" s="2">
         <v>1977</v>
       </c>
       <c r="B1977" s="1" t="s">
         <v>1975</v>
       </c>
-    </row>
-    <row r="1978" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1977" s="1" t="s">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1978" s="2">
         <v>1978</v>
       </c>
@@ -25682,7 +25731,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="1979" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1979" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1979" s="2">
         <v>1979</v>
       </c>
@@ -25690,7 +25739,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="1980" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1980" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1980" s="2">
         <v>1980</v>
       </c>
@@ -25698,7 +25747,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="1981" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1981" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1981" s="2">
         <v>1981</v>
       </c>
@@ -25706,7 +25755,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="1982" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1982" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1982" s="2">
         <v>1982</v>
       </c>
@@ -25714,7 +25763,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="1983" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1983" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1983" s="2">
         <v>1983</v>
       </c>
@@ -25722,7 +25771,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="1984" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1984" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1984" s="2">
         <v>1984</v>
       </c>
@@ -25858,7 +25907,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="2001" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2001" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2001" s="2">
         <v>2001</v>
       </c>
@@ -25866,7 +25915,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="2002" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2002" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2002" s="2">
         <v>2002</v>
       </c>
@@ -25874,7 +25923,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="2003" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2003" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2003" s="2">
         <v>2003</v>
       </c>
@@ -25882,7 +25931,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="2004" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2004" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2004" s="2">
         <v>2004</v>
       </c>
@@ -25890,7 +25939,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="2005" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2005" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2005" s="2">
         <v>2005</v>
       </c>
@@ -25898,7 +25947,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="2006" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2006" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2006" s="2">
         <v>2006</v>
       </c>
@@ -25906,7 +25955,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="2007" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2007" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2007" s="2">
         <v>2007</v>
       </c>
@@ -25914,7 +25963,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="2008" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2008" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2008" s="2">
         <v>2008</v>
       </c>
@@ -25922,7 +25971,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="2009" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2009" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2009" s="2">
         <v>2009</v>
       </c>
@@ -25930,7 +25979,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="2010" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2010" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2010" s="2">
         <v>2010</v>
       </c>
@@ -25938,15 +25987,18 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="2011" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2011" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2011" s="2">
         <v>2011</v>
       </c>
       <c r="B2011" s="1" t="s">
         <v>2009</v>
       </c>
-    </row>
-    <row r="2012" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2011" s="1" t="s">
+        <v>3174</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2012" s="2">
         <v>2012</v>
       </c>
@@ -25954,7 +26006,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="2013" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2013" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2013" s="2">
         <v>2013</v>
       </c>
@@ -25962,7 +26014,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="2014" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2014" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2014" s="2">
         <v>2014</v>
       </c>
@@ -25970,7 +26022,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="2015" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2015" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2015" s="2">
         <v>2015</v>
       </c>
@@ -25978,7 +26030,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="2016" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2016" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2016" s="2">
         <v>2016</v>
       </c>
@@ -26498,7 +26550,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="2081" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2081" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2081" s="2">
         <v>2081</v>
       </c>
@@ -26506,7 +26558,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="2082" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2082" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2082" s="2">
         <v>2082</v>
       </c>
@@ -26514,7 +26566,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="2083" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2083" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2083" s="2">
         <v>2083</v>
       </c>
@@ -26522,7 +26574,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="2084" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2084" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2084" s="2">
         <v>2084</v>
       </c>
@@ -26530,7 +26582,7 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="2085" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2085" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2085" s="2">
         <v>2085</v>
       </c>
@@ -26538,7 +26590,7 @@
         <v>2083</v>
       </c>
     </row>
-    <row r="2086" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2086" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2086" s="2">
         <v>2086</v>
       </c>
@@ -26546,7 +26598,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="2087" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2087" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2087" s="2">
         <v>2087</v>
       </c>
@@ -26554,7 +26606,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="2088" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2088" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2088" s="2">
         <v>2088</v>
       </c>
@@ -26562,15 +26614,18 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="2089" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2089" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2089" s="2">
         <v>2089</v>
       </c>
       <c r="B2089" s="1" t="s">
         <v>2087</v>
       </c>
-    </row>
-    <row r="2090" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2089" s="1" t="s">
+        <v>3172</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2090" s="2">
         <v>2090</v>
       </c>
@@ -26578,7 +26633,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="2091" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2091" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2091" s="2">
         <v>2091</v>
       </c>
@@ -26586,7 +26641,7 @@
         <v>2089</v>
       </c>
     </row>
-    <row r="2092" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2092" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2092" s="2">
         <v>2092</v>
       </c>
@@ -26594,7 +26649,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="2093" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2093" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2093" s="2">
         <v>2093</v>
       </c>
@@ -26602,7 +26657,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="2094" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2094" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2094" s="2">
         <v>2094</v>
       </c>
@@ -26610,7 +26665,7 @@
         <v>2092</v>
       </c>
     </row>
-    <row r="2095" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2095" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2095" s="2">
         <v>2095</v>
       </c>
@@ -26618,7 +26673,7 @@
         <v>2093</v>
       </c>
     </row>
-    <row r="2096" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2096" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2096" s="2">
         <v>2096</v>
       </c>
@@ -31362,7 +31417,7 @@
         <v>2686</v>
       </c>
     </row>
-    <row r="2689" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2689" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2689" s="2">
         <v>2689</v>
       </c>
@@ -31370,7 +31425,7 @@
         <v>2687</v>
       </c>
     </row>
-    <row r="2690" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2690" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2690" s="2">
         <v>2690</v>
       </c>
@@ -31378,7 +31433,7 @@
         <v>2688</v>
       </c>
     </row>
-    <row r="2691" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2691" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2691" s="2">
         <v>2691</v>
       </c>
@@ -31386,7 +31441,7 @@
         <v>2689</v>
       </c>
     </row>
-    <row r="2692" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2692" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2692" s="2">
         <v>2692</v>
       </c>
@@ -31394,7 +31449,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="2693" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2693" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2693" s="2">
         <v>2693</v>
       </c>
@@ -31402,7 +31457,7 @@
         <v>2691</v>
       </c>
     </row>
-    <row r="2694" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2694" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2694" s="2">
         <v>2694</v>
       </c>
@@ -31410,7 +31465,7 @@
         <v>2692</v>
       </c>
     </row>
-    <row r="2695" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2695" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2695" s="2">
         <v>2695</v>
       </c>
@@ -31418,7 +31473,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="2696" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2696" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2696" s="2">
         <v>2696</v>
       </c>
@@ -31426,15 +31481,18 @@
         <v>2694</v>
       </c>
     </row>
-    <row r="2697" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2697" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2697" s="2">
         <v>2697</v>
       </c>
       <c r="B2697" s="1" t="s">
         <v>2695</v>
       </c>
-    </row>
-    <row r="2698" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2697" s="1" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2698" s="2">
         <v>2698</v>
       </c>
@@ -31442,7 +31500,7 @@
         <v>2696</v>
       </c>
     </row>
-    <row r="2699" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2699" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2699" s="2">
         <v>2699</v>
       </c>
@@ -31450,7 +31508,7 @@
         <v>2697</v>
       </c>
     </row>
-    <row r="2700" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2700" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2700" s="2">
         <v>2700</v>
       </c>
@@ -31458,7 +31516,7 @@
         <v>2698</v>
       </c>
     </row>
-    <row r="2701" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2701" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2701" s="2">
         <v>2701</v>
       </c>
@@ -31466,7 +31524,7 @@
         <v>2699</v>
       </c>
     </row>
-    <row r="2702" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2702" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2702" s="2">
         <v>2702</v>
       </c>
@@ -31474,7 +31532,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="2703" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2703" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2703" s="2">
         <v>2703</v>
       </c>
@@ -31482,7 +31540,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="2704" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2704" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2704" s="2">
         <v>2704</v>
       </c>
@@ -34562,7 +34620,7 @@
         <v>3086</v>
       </c>
     </row>
-    <row r="3089" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3089" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3089" s="2">
         <v>3089</v>
       </c>
@@ -34570,7 +34628,7 @@
         <v>3087</v>
       </c>
     </row>
-    <row r="3090" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3090" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3090" s="2">
         <v>3090</v>
       </c>
@@ -34578,7 +34636,7 @@
         <v>3088</v>
       </c>
     </row>
-    <row r="3091" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3091" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3091" s="2">
         <v>3091</v>
       </c>
@@ -34586,7 +34644,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="3092" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3092" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3092" s="2">
         <v>3092</v>
       </c>
@@ -34594,7 +34652,7 @@
         <v>3090</v>
       </c>
     </row>
-    <row r="3093" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3093" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3093" s="2">
         <v>3093</v>
       </c>
@@ -34602,7 +34660,7 @@
         <v>3091</v>
       </c>
     </row>
-    <row r="3094" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3094" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3094" s="2">
         <v>3094</v>
       </c>
@@ -34610,7 +34668,7 @@
         <v>3092</v>
       </c>
     </row>
-    <row r="3095" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3095" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3095" s="2">
         <v>3095</v>
       </c>
@@ -34618,7 +34676,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="3096" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3096" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3096" s="2">
         <v>3096</v>
       </c>
@@ -34626,7 +34684,7 @@
         <v>3094</v>
       </c>
     </row>
-    <row r="3097" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3097" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3097" s="2">
         <v>3097</v>
       </c>
@@ -34634,7 +34692,7 @@
         <v>3095</v>
       </c>
     </row>
-    <row r="3098" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3098" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3098" s="2">
         <v>3098</v>
       </c>
@@ -34642,7 +34700,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="3099" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3099" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3099" s="2">
         <v>3099</v>
       </c>
@@ -34650,7 +34708,7 @@
         <v>3097</v>
       </c>
     </row>
-    <row r="3100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3100" s="2">
         <v>3100</v>
       </c>
@@ -34658,7 +34716,7 @@
         <v>3098</v>
       </c>
     </row>
-    <row r="3101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3101" s="2">
         <v>3101</v>
       </c>
@@ -34666,7 +34724,7 @@
         <v>3099</v>
       </c>
     </row>
-    <row r="3102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3102" s="2">
         <v>3102</v>
       </c>
@@ -34674,15 +34732,18 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="3103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3103" s="2">
         <v>3103</v>
       </c>
       <c r="B3103" s="1" t="s">
         <v>3101</v>
       </c>
-    </row>
-    <row r="3104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3103" s="1" t="s">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="3104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3104" s="2">
         <v>3104</v>
       </c>

</xml_diff>